<commit_message>
Detaily k poslaní příkladů.
</commit_message>
<xml_diff>
--- a/evidence uzivatelu/Cars.xlsx
+++ b/evidence uzivatelu/Cars.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -23,22 +23,10 @@
     <t>Škoda</t>
   </si>
   <si>
-    <t>Renoult</t>
-  </si>
-  <si>
-    <t>Peugeot</t>
-  </si>
-  <si>
     <t>SPZ</t>
   </si>
   <si>
     <t>BAC15973</t>
-  </si>
-  <si>
-    <t>sss 12345</t>
-  </si>
-  <si>
-    <t>asd78945</t>
   </si>
   <si>
     <t>Cena</t>
@@ -71,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -100,20 +88,31 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" borderId="2" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" borderId="3" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="3" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="2" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="4" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="5" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -124,7 +123,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -134,70 +133,40 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="4">
         <v>0</v>
-      </c>
-      <c r="C1" s="6">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="0" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>8</v>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="0">
         <v>40000</v>
-      </c>
-      <c r="C4" s="5">
-        <v>200000</v>
-      </c>
-      <c r="D4" s="8">
-        <v>120000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>9458</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>